<commit_message>
Clean up dirs, rename main python file, fix issue with uppercase naming in risks
</commit_message>
<xml_diff>
--- a/output/risks.xlsx
+++ b/output/risks.xlsx
@@ -172,10 +172,7 @@
     <t>Missing Cloud Hardening</t>
   </si>
   <si>
-    <t>SSPHP-Metrics</t>
-  </si>
-  <si>
-    <t>Missing Cloud Hardening (Azure) risk at SSPHP-Metrics: CIS Benchmark for Microsoft Azure</t>
+    <t>Missing Cloud Hardening (Azure) risk at s184d01-comp-complete-app: CIS Benchmark for Microsoft Azure</t>
   </si>
   <si>
     <t>Cloud Hardening</t>
@@ -184,7 +181,7 @@
     <t>Apply hardening of all cloud components and services, taking special care to follow the individual risk descriptions (which depend on the cloud provider tags in the model). &lt;br&gt;&lt;br&gt;For &lt;b&gt;Amazon Web Services (AWS)&lt;/b&gt;: Follow the &lt;i&gt;CIS Benchmark for Amazon Web Services&lt;/i&gt; (see also the automated checks of cloud audit tools like &lt;i&gt;"PacBot", "CloudSploit", "CloudMapper", "ScoutSuite", or "Prowler AWS CIS Benchmark Tool"&lt;/i&gt;). &lt;br&gt;For EC2 and other servers running Amazon Linux, follow the &lt;i&gt;CIS Benchmark for Amazon Linux&lt;/i&gt; and switch to IMDSv2. &lt;br&gt;For S3 buckets follow the &lt;i&gt;Security Best Practices for Amazon S3&lt;/i&gt; at &lt;a href="https://docs.aws.amazon.com/AmazonS3/latest/dev/security-best-practices.html"&gt;https://docs.aws.amazon.com/AmazonS3/latest/dev/security-best-practices.html&lt;/a&gt; to avoid accidental leakage. &lt;br&gt;Also take a look at some of these tools: &lt;a href="https://github.com/toniblyx/my-arsenal-of-aws-security-tools"&gt;https://github.com/toniblyx/my-arsenal-of-aws-security-tools&lt;/a&gt; &lt;br&gt;&lt;br&gt;For &lt;b&gt;Microsoft Azure&lt;/b&gt;: Follow the &lt;i&gt;CIS Benchmark for Microsoft Azure&lt;/i&gt; (see also the automated checks of cloud audit tools like &lt;i&gt;"CloudSploit" or "ScoutSuite"&lt;/i&gt;).&lt;br&gt;&lt;br&gt;For &lt;b&gt;Google Cloud Platform&lt;/b&gt;: Follow the &lt;i&gt;CIS Benchmark for Google Cloud Computing Platform&lt;/i&gt; (see also the automated checks of cloud audit tools like &lt;i&gt;"CloudSploit" or "ScoutSuite"&lt;/i&gt;). &lt;br&gt;&lt;br&gt;For &lt;b&gt;Oracle Cloud Platform&lt;/b&gt;: Follow the hardening best practices (see also the automated checks of cloud audit tools like &lt;i&gt;"CloudSploit"&lt;/i&gt;).</t>
   </si>
   <si>
-    <t>missing-cloud-hardening@SSPHP-Metrics</t>
+    <t>missing-cloud-hardening@s184d01-comp-complete-app</t>
   </si>
   <si>
     <t>Low</t>
@@ -196,7 +193,10 @@
     <t>Missing Hardening</t>
   </si>
   <si>
-    <t>Missing Hardening risk at SSPHP-Metrics</t>
+    <t>s184d01-comp-tfvars</t>
+  </si>
+  <si>
+    <t>Missing Hardening risk at s184d01-comp-tfvars</t>
   </si>
   <si>
     <t>System Hardening</t>
@@ -205,25 +205,25 @@
     <t>Try to apply all hardening best practices (like CIS benchmarks, OWASP recommendations, vendor recommendations, DevSec Hardening Framework, DBSAT for Oracle databases, and others).</t>
   </si>
   <si>
-    <t>missing-hardening@SSPHP-Metrics</t>
-  </si>
-  <si>
-    <t>s184d01-comp-tfvars</t>
-  </si>
-  <si>
-    <t>Missing Hardening risk at s184d01-comp-tfvars</t>
-  </si>
-  <si>
     <t>missing-hardening@s184d01-comp-tfvars</t>
   </si>
   <si>
+    <t>ssphp-metrics</t>
+  </si>
+  <si>
+    <t>Missing Hardening risk at ssphp-metrics</t>
+  </si>
+  <si>
+    <t>missing-hardening@ssphp-metrics</t>
+  </si>
+  <si>
     <t>Elevation of Privilege</t>
   </si>
   <si>
     <t>Missing Vault Isolation</t>
   </si>
   <si>
-    <t>Missing Vault Isolation to further encapsulate and protect vault-related asset SSPHP-Metrics against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
+    <t>Missing Vault Isolation to further encapsulate and protect vault-related asset s184d01-comp-tfvars against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
   </si>
   <si>
     <t>Network Segmentation</t>
@@ -232,15 +232,15 @@
     <t>Apply a network segmentation trust-boundary around the highly sensitive vault assets and their datastores.</t>
   </si>
   <si>
-    <t>missing-vault-isolation@SSPHP-Metrics</t>
-  </si>
-  <si>
-    <t>Missing Vault Isolation to further encapsulate and protect vault-related asset s184d01-comp-tfvars against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
-  </si>
-  <si>
     <t>missing-vault-isolation@s184d01-comp-tfvars</t>
   </si>
   <si>
+    <t>Missing Vault Isolation to further encapsulate and protect vault-related asset ssphp-metrics against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
+  </si>
+  <si>
+    <t>missing-vault-isolation@ssphp-metrics</t>
+  </si>
+  <si>
     <t>Information Disclosure</t>
   </si>
   <si>
@@ -250,10 +250,7 @@
     <t>Unencrypted Technical Assets</t>
   </si>
   <si>
-    <t>SSPHP-Metrics-rust-p3sha</t>
-  </si>
-  <si>
-    <t>Unencrypted Technical Asset named SSPHP-Metrics-rust-p3sha</t>
+    <t>Unencrypted Technical Asset named s184d01-comp-complete-app-worker</t>
   </si>
   <si>
     <t>Encryption of Technical Asset</t>
@@ -262,18 +259,6 @@
     <t>Apply encryption to the technical asset.</t>
   </si>
   <si>
-    <t>unencrypted-asset@SSPHP-Metrics-rust-p3sha</t>
-  </si>
-  <si>
-    <t>Unencrypted Technical Asset named SSPHP-Metrics</t>
-  </si>
-  <si>
-    <t>unencrypted-asset@SSPHP-Metrics</t>
-  </si>
-  <si>
-    <t>Unencrypted Technical Asset named s184d01-comp-complete-app-worker</t>
-  </si>
-  <si>
     <t>unencrypted-asset@s184d01-comp-complete-app-worker</t>
   </si>
   <si>
@@ -298,6 +283,21 @@
     <t>unencrypted-asset@s184d01-compdefault</t>
   </si>
   <si>
+    <t>ssphp-metrics-rust-p3sha</t>
+  </si>
+  <si>
+    <t>Unencrypted Technical Asset named ssphp-metrics-rust-p3sha</t>
+  </si>
+  <si>
+    <t>unencrypted-asset@ssphp-metrics-rust-p3sha</t>
+  </si>
+  <si>
+    <t>Unencrypted Technical Asset named ssphp-metrics</t>
+  </si>
+  <si>
+    <t>unencrypted-asset@ssphp-metrics</t>
+  </si>
+  <si>
     <t>tfstatel95cd</t>
   </si>
   <si>
@@ -319,21 +319,21 @@
     <t>Missing Network Segmentation</t>
   </si>
   <si>
-    <t>Missing Network Segmentation to further encapsulate and protect SSPHP-Metrics against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
+    <t>Missing Network Segmentation to further encapsulate and protect s184d01-comp-tfvars against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
   </si>
   <si>
     <t>Apply a network segmentation trust-boundary around the highly sensitive assets and/or datastores.</t>
   </si>
   <si>
-    <t>missing-network-segmentation@SSPHP-Metrics</t>
-  </si>
-  <si>
-    <t>Missing Network Segmentation to further encapsulate and protect s184d01-comp-tfvars against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
-  </si>
-  <si>
     <t>missing-network-segmentation@s184d01-comp-tfvars</t>
   </si>
   <si>
+    <t>Missing Network Segmentation to further encapsulate and protect ssphp-metrics against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
+  </si>
+  <si>
+    <t>missing-network-segmentation@ssphp-metrics</t>
+  </si>
+  <si>
     <t>Architecture</t>
   </si>
   <si>
@@ -403,24 +403,12 @@
     <t>Unnecessary Technical Asset</t>
   </si>
   <si>
-    <t>Unnecessary Technical Asset named SSPHP-Metrics-rust-p3sha</t>
+    <t>Unnecessary Technical Asset named s184d01-comp-complete-app-worker</t>
   </si>
   <si>
     <t>Try to avoid using technical assets that do not process or store anything.</t>
   </si>
   <si>
-    <t>unnecessary-technical-asset@SSPHP-Metrics-rust-p3sha</t>
-  </si>
-  <si>
-    <t>Unnecessary Technical Asset named SSPHP-Metrics</t>
-  </si>
-  <si>
-    <t>unnecessary-technical-asset@SSPHP-Metrics</t>
-  </si>
-  <si>
-    <t>Unnecessary Technical Asset named s184d01-comp-complete-app-worker</t>
-  </si>
-  <si>
     <t>unnecessary-technical-asset@s184d01-comp-complete-app-worker</t>
   </si>
   <si>
@@ -440,6 +428,18 @@
   </si>
   <si>
     <t>unnecessary-technical-asset@s184d01-compdefault</t>
+  </si>
+  <si>
+    <t>Unnecessary Technical Asset named ssphp-metrics-rust-p3sha</t>
+  </si>
+  <si>
+    <t>unnecessary-technical-asset@ssphp-metrics-rust-p3sha</t>
+  </si>
+  <si>
+    <t>Unnecessary Technical Asset named ssphp-metrics</t>
+  </si>
+  <si>
+    <t>unnecessary-technical-asset@ssphp-metrics</t>
   </si>
   <si>
     <t>Unnecessary Technical Asset named tfstatel95cd</t>
@@ -1286,28 +1286,28 @@
         <v>51</v>
       </c>
       <c r="H6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="18">
+        <v>1</v>
+      </c>
+      <c r="K6" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="18">
-        <v>100</v>
-      </c>
-      <c r="K6" s="19" t="s">
+      <c r="L6" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="L6" s="22" t="s">
+      <c r="M6" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="22" t="s">
+      <c r="N6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="20" t="s">
         <v>55</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O6" s="20" t="s">
-        <v>56</v>
       </c>
       <c r="P6" s="10" t="s">
         <v>34</v>
@@ -1325,7 +1325,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>23</v>
@@ -1334,13 +1334,13 @@
         <v>39</v>
       </c>
       <c r="F7" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>28</v>
@@ -1379,7 +1379,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>23</v>
@@ -1388,10 +1388,10 @@
         <v>39</v>
       </c>
       <c r="F8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>64</v>
@@ -1448,7 +1448,7 @@
         <v>68</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>28</v>
@@ -1556,7 +1556,7 @@
         <v>77</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>28</v>
@@ -1565,19 +1565,19 @@
         <v>1</v>
       </c>
       <c r="K11" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="L11" s="22" t="s">
+      <c r="M11" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="M11" s="22" t="s">
+      <c r="N11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11" s="20" t="s">
         <v>81</v>
-      </c>
-      <c r="N11" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O11" s="20" t="s">
-        <v>82</v>
       </c>
       <c r="P11" s="10" t="s">
         <v>34</v>
@@ -1610,28 +1610,28 @@
         <v>77</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J12" s="18">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="K12" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" s="20" t="s">
         <v>83</v>
-      </c>
-      <c r="L12" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="M12" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="N12" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O12" s="20" t="s">
-        <v>84</v>
       </c>
       <c r="P12" s="10" t="s">
         <v>34</v>
@@ -1664,28 +1664,28 @@
         <v>77</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J13" s="18">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="K13" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="N13" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" s="20" t="s">
         <v>85</v>
-      </c>
-      <c r="L13" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="M13" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="N13" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O13" s="20" t="s">
-        <v>86</v>
       </c>
       <c r="P13" s="10" t="s">
         <v>34</v>
@@ -1718,7 +1718,7 @@
         <v>77</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>28</v>
@@ -1730,10 +1730,10 @@
         <v>87</v>
       </c>
       <c r="L14" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="M14" s="22" t="s">
         <v>80</v>
-      </c>
-      <c r="M14" s="22" t="s">
-        <v>81</v>
       </c>
       <c r="N14" s="22" t="s">
         <v>32</v>
@@ -1772,28 +1772,28 @@
         <v>77</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J15" s="18">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L15" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="M15" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="M15" s="22" t="s">
-        <v>81</v>
-      </c>
       <c r="N15" s="22" t="s">
         <v>32</v>
       </c>
       <c r="O15" s="20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="P15" s="10" t="s">
         <v>34</v>
@@ -1826,22 +1826,22 @@
         <v>77</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J16" s="18">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="K16" s="19" t="s">
         <v>92</v>
       </c>
       <c r="L16" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="M16" s="22" t="s">
         <v>80</v>
-      </c>
-      <c r="M16" s="22" t="s">
-        <v>81</v>
       </c>
       <c r="N16" s="22" t="s">
         <v>32</v>
@@ -1892,10 +1892,10 @@
         <v>95</v>
       </c>
       <c r="L17" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="M17" s="22" t="s">
         <v>80</v>
-      </c>
-      <c r="M17" s="22" t="s">
-        <v>81</v>
       </c>
       <c r="N17" s="22" t="s">
         <v>32</v>
@@ -1946,10 +1946,10 @@
         <v>98</v>
       </c>
       <c r="L18" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="M18" s="22" t="s">
         <v>80</v>
-      </c>
-      <c r="M18" s="22" t="s">
-        <v>81</v>
       </c>
       <c r="N18" s="22" t="s">
         <v>32</v>
@@ -1967,13 +1967,13 @@
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>67</v>
@@ -1988,7 +1988,7 @@
         <v>100</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>28</v>
@@ -2021,13 +2021,13 @@
     </row>
     <row r="20">
       <c r="A20" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>67</v>
@@ -2075,13 +2075,13 @@
     </row>
     <row r="21">
       <c r="A21" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>67</v>
@@ -2129,13 +2129,13 @@
     </row>
     <row r="22">
       <c r="A22" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>67</v>
@@ -2183,13 +2183,13 @@
     </row>
     <row r="23">
       <c r="A23" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>67</v>
@@ -2237,13 +2237,13 @@
     </row>
     <row r="24">
       <c r="A24" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>67</v>
@@ -2291,13 +2291,13 @@
     </row>
     <row r="25">
       <c r="A25" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>67</v>
@@ -2345,13 +2345,13 @@
     </row>
     <row r="26">
       <c r="A26" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>67</v>
@@ -2399,13 +2399,13 @@
     </row>
     <row r="27">
       <c r="A27" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>67</v>
@@ -2453,13 +2453,13 @@
     </row>
     <row r="28">
       <c r="A28" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>67</v>
@@ -2507,13 +2507,13 @@
     </row>
     <row r="29">
       <c r="A29" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>67</v>
@@ -2561,13 +2561,13 @@
     </row>
     <row r="30">
       <c r="A30" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>67</v>
@@ -2582,7 +2582,7 @@
         <v>128</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="I30" s="9" t="s">
         <v>28</v>
@@ -2615,13 +2615,13 @@
     </row>
     <row r="31">
       <c r="A31" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>67</v>
@@ -2636,13 +2636,13 @@
         <v>128</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="I31" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J31" s="18">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="K31" s="19" t="s">
         <v>132</v>
@@ -2669,13 +2669,13 @@
     </row>
     <row r="32">
       <c r="A32" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>67</v>
@@ -2690,13 +2690,13 @@
         <v>128</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="I32" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J32" s="18">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="K32" s="19" t="s">
         <v>134</v>
@@ -2723,13 +2723,13 @@
     </row>
     <row r="33">
       <c r="A33" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>67</v>
@@ -2744,7 +2744,7 @@
         <v>128</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="I33" s="9" t="s">
         <v>28</v>
@@ -2777,13 +2777,13 @@
     </row>
     <row r="34">
       <c r="A34" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>67</v>
@@ -2798,13 +2798,13 @@
         <v>128</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J34" s="18">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="K34" s="19" t="s">
         <v>138</v>
@@ -2831,13 +2831,13 @@
     </row>
     <row r="35">
       <c r="A35" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>67</v>
@@ -2852,13 +2852,13 @@
         <v>128</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="I35" s="9" t="s">
         <v>28</v>
       </c>
       <c r="J35" s="18">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="K35" s="19" t="s">
         <v>140</v>
@@ -2885,13 +2885,13 @@
     </row>
     <row r="36">
       <c r="A36" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>67</v>
@@ -2939,13 +2939,13 @@
     </row>
     <row r="37">
       <c r="A37" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>67</v>

</xml_diff>